<commit_message>
all test cases ready except for combined production
</commit_message>
<xml_diff>
--- a/test_cases/recalculation - circular reference.xlsx
+++ b/test_cases/recalculation - circular reference.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meta!$A$1:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">quantitative!$A$1:$U$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">quantitative!$A$1:$U$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>access restricted</t>
   </si>
@@ -61,9 +61,6 @@
     <t>technology level</t>
   </si>
   <si>
-    <t>test case economic allocation</t>
-  </si>
-  <si>
     <t>GLO</t>
   </si>
   <si>
@@ -157,12 +154,6 @@
     <t>uncertainty type</t>
   </si>
   <si>
-    <t>production volume</t>
-  </si>
-  <si>
-    <t>parameters</t>
-  </si>
-  <si>
     <t>exchange id</t>
   </si>
   <si>
@@ -172,9 +163,6 @@
     <t>parameter id</t>
   </si>
   <si>
-    <t>properties</t>
-  </si>
-  <si>
     <t>field</t>
   </si>
   <si>
@@ -184,121 +172,49 @@
     <t>exchange_01</t>
   </si>
   <si>
-    <t>exchange_02</t>
-  </si>
-  <si>
-    <t>exchange_03</t>
-  </si>
-  <si>
-    <t>byproduct</t>
-  </si>
-  <si>
-    <t>from technosphere</t>
-  </si>
-  <si>
-    <t>from environment</t>
-  </si>
-  <si>
-    <t>to environment</t>
-  </si>
-  <si>
-    <t>exchange_04</t>
-  </si>
-  <si>
-    <t>exchange_05</t>
-  </si>
-  <si>
-    <t>parameter_01</t>
-  </si>
-  <si>
-    <t>heat</t>
-  </si>
-  <si>
-    <t>coal</t>
-  </si>
-  <si>
-    <t>carbon dioxide, fossil</t>
-  </si>
-  <si>
-    <t>cooling water</t>
-  </si>
-  <si>
-    <t>natural resource</t>
-  </si>
-  <si>
-    <t>in water</t>
-  </si>
-  <si>
-    <t>air</t>
-  </si>
-  <si>
-    <t>unspecified</t>
-  </si>
-  <si>
     <t>allocatable</t>
   </si>
   <si>
     <t>kWh</t>
   </si>
   <si>
-    <t>MJ</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>var1</t>
-  </si>
-  <si>
-    <t>var3</t>
-  </si>
-  <si>
-    <t>var5</t>
-  </si>
-  <si>
-    <t>var2</t>
-  </si>
-  <si>
-    <t>var4</t>
-  </si>
-  <si>
-    <t>var6</t>
-  </si>
-  <si>
-    <t>var7</t>
-  </si>
-  <si>
-    <t>var8</t>
-  </si>
-  <si>
-    <t>var9</t>
-  </si>
-  <si>
-    <t>var10</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>EURO2005</t>
-  </si>
-  <si>
-    <t>var11</t>
-  </si>
-  <si>
-    <t>true value relation</t>
-  </si>
-  <si>
     <t>dataset_01</t>
   </si>
   <si>
-    <t>yield</t>
-  </si>
-  <si>
-    <t>adimensional</t>
+    <t>recalculation - circular reference</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>parameter 1</t>
+  </si>
+  <si>
+    <t>par_1</t>
+  </si>
+  <si>
+    <t>parameter 2</t>
+  </si>
+  <si>
+    <t>par_1*2</t>
+  </si>
+  <si>
+    <t>par_2</t>
+  </si>
+  <si>
+    <t>parameter 3</t>
+  </si>
+  <si>
+    <t>par_2*9</t>
+  </si>
+  <si>
+    <t>par_3</t>
+  </si>
+  <si>
+    <t>par_3*3</t>
   </si>
 </sst>
 </file>
@@ -630,7 +546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,18 +556,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -667,15 +583,15 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -683,7 +599,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -691,15 +607,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -707,7 +623,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -715,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -731,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -743,10 +659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,366 +676,154 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>29</v>
-      </c>
       <c r="O1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>39</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
         <v>36</v>
-      </c>
-      <c r="S1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" t="s">
-        <v>68</v>
-      </c>
       <c r="K3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>49</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
       </c>
       <c r="N3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
       <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>71</v>
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7">
-        <v>50000</v>
-      </c>
-      <c r="L7" t="s">
-        <v>69</v>
-      </c>
-      <c r="N7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
         <v>60</v>
       </c>
-      <c r="J8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8">
-        <v>15000</v>
-      </c>
-      <c r="L8" t="s">
-        <v>70</v>
-      </c>
-      <c r="N8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" t="s">
-        <v>68</v>
-      </c>
-      <c r="K9">
-        <v>5</v>
-      </c>
-      <c r="L9" t="s">
-        <v>84</v>
-      </c>
-      <c r="N9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10">
-        <v>4</v>
-      </c>
-      <c r="L10" t="s">
-        <v>84</v>
-      </c>
-      <c r="N10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" t="s">
-        <v>88</v>
-      </c>
-      <c r="K11">
-        <v>0.11</v>
-      </c>
-      <c r="L11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12">
-        <v>11</v>
-      </c>
-      <c r="L12" t="s">
-        <v>89</v>
-      </c>
-      <c r="N12" t="s">
-        <v>85</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U7"/>
+  <autoFilter ref="A1:U5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>